<commit_message>
Some formatting updates to GAM code, GAM figures, and metadata
</commit_message>
<xml_diff>
--- a/metadata/p1969RiverWaterCB_metadata.xlsx
+++ b/metadata/p1969RiverWaterCB_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Camryn\Documents\NC-Ecosystem-indicators\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BECFEC86-A8E4-4E16-9EBA-02F9A3373F10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A7A429-1C4E-46CD-AAEC-1FE02BEFB79C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2120" yWindow="2120" windowWidth="14400" windowHeight="8170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata Form" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Datset File Name:</t>
   </si>
@@ -98,11 +98,6 @@
     <t>NCDENR-DWQ</t>
   </si>
   <si>
-    <t>North Carolina Department of Environmental Quality
-217 West Jones Street
-Raleigh, NC 27603</t>
-  </si>
-  <si>
     <t xml:space="preserve">Water Quality Portal. Washington (DC): National Water Quality Monitoring Council, United States Geological Survey (USGS), Environmental Protection Agency (EPA); 2021. https://doi.org/10.5066/P9QRKUVJ. </t>
   </si>
   <si>
@@ -119,6 +114,39 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>North Carolina Department of Environmental Resources NCDENR-DWQ WQX</t>
+  </si>
+  <si>
+    <t>State of North Carolina, Department of Environment and Natural Resources.</t>
+  </si>
+  <si>
+    <t>*State Government US</t>
+  </si>
+  <si>
+    <t>mark.hale@ncdenr.gov (Email);brian.pointer@ncdenr.gov (Email)</t>
+  </si>
+  <si>
+    <t>919-743-8400 (Office)</t>
+  </si>
+  <si>
+    <t>Mailing</t>
+  </si>
+  <si>
+    <t>1621 Mail Service Center</t>
+  </si>
+  <si>
+    <t>For mail only</t>
+  </si>
+  <si>
+    <t>Raleigh</t>
+  </si>
+  <si>
+    <t>NC</t>
+  </si>
+  <si>
+    <t>27699-1621</t>
   </si>
 </sst>
 </file>
@@ -181,12 +209,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -405,8 +431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -581,20 +607,40 @@
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>23</v>
+      <c r="B6" s="6" t="s">
+        <v>29</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
+      <c r="C6" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>39</v>
+      </c>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
@@ -613,7 +659,7 @@
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C7" s="2"/>
@@ -646,7 +692,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -678,7 +724,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -742,7 +788,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -774,7 +820,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -806,7 +852,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -838,7 +884,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>

</xml_diff>